<commit_message>
In BOM, changed .47uF capacitor to one with .55mm thickness
</commit_message>
<xml_diff>
--- a/killswitch/killswitch_BOM.xlsx
+++ b/killswitch/killswitch_BOM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$2</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Part Description</t>
   </si>
@@ -151,16 +151,28 @@
   </si>
   <si>
     <t>The output Terminal 3-pin is actually in the projects club and does not need to be purchased.</t>
+  </si>
+  <si>
+    <t>CGB3B3X5R1E474K055AB</t>
+  </si>
+  <si>
+    <t>445-13240-1-ND</t>
+  </si>
+  <si>
+    <t>https://product.tdk.com/info/en/catalog/spec/mlccspec_commercial_lowprofile_en.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/tdk-corporation/CGB3B3X5R1E474K055AB/445-13240-1-ND/3954906</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +209,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,14 +259,11 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -247,8 +271,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -530,11 +563,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,54 +577,54 @@
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="6" width="27.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="7" customWidth="1"/>
     <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="8" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="7" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -602,31 +635,31 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>3.8</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <f>SUMPRODUCT(G3,H3)</f>
         <v>3.8</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="7">
         <f ca="1">SUM(OFFSET(I3,0,0,ROWS(I:I)-ROW(I3)+1))</f>
-        <v>17.477999999999998</v>
+        <v>18.114000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -636,10 +669,10 @@
       <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
@@ -648,13 +681,13 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>1.59</v>
       </c>
       <c r="H4">
         <v>4</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <f>SUMPRODUCT(G4,H4)</f>
         <v>6.36</v>
       </c>
@@ -666,10 +699,10 @@
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E5" t="s">
@@ -678,13 +711,13 @@
       <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>1.73</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <f>SUMPRODUCT(G5,H5)</f>
         <v>6.92</v>
       </c>
@@ -696,10 +729,10 @@
       <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E6" t="s">
@@ -708,45 +741,72 @@
       <c r="F6" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <f>SUMPRODUCT(G6,H6)</f>
         <v>0.19</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="12">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="9">
         <v>4</v>
       </c>
-      <c r="I7" s="8">
-        <f>SUMPRODUCT(G7,H7)</f>
-        <v>0.20799999999999999</v>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8" s="7">
+        <f>SUMPRODUCT(G8,H8)</f>
+        <v>0.84399999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -768,14 +828,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I2" xr:uid="{19FFC98B-5891-4144-AC08-C807834125D2}"/>
+  <autoFilter ref="A2:I2"/>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{63F50D71-822D-472E-AB7C-7E6193081B39}"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="E8" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>